<commit_message>
Built a prototype of the app working fine
</commit_message>
<xml_diff>
--- a/Auto_Prescription_App/Medical_Records.xlsx
+++ b/Auto_Prescription_App/Medical_Records.xlsx
@@ -1,74 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOGOL\Documents\My Projects copy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342B6357-6BD1-4585-8A32-38DD3D116FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="1515" windowWidth="14010" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="885" yWindow="1515" windowWidth="14010" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Date-Time</t>
-  </si>
-  <si>
-    <t>History with complaints</t>
-  </si>
-  <si>
-    <t>Clinical Findings</t>
-  </si>
-  <si>
-    <t>Investigations</t>
-  </si>
-  <si>
-    <t>advice_to_follow</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -87,23 +53,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -423,56 +448,154 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col width="9.85546875" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="5.5703125" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="5.28515625" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="13" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="26.140625" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
+    <col width="27.140625" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+    <row r="1" ht="18.75" customHeight="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date-Time</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>History with complaints</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Clinical Findings</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Investigations</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>advice_to_follow</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>subhra Bala</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>05-01-2025 16:10:46</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>sdfsdfsdgsdg</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>sdgsdgsdgsd</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>gweawegasegasd</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>gasdgasdgas</t>
+        </is>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Subhra Bala</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>05-01-2025 16:21:56</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Yes yes yes</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>No No No</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
made some slight changes to the auto prescription app, bascially changed the docx and pdf file location to same directory as that of the main app
</commit_message>
<xml_diff>
--- a/Auto_Prescription_App/Medical_Records.xlsx
+++ b/Auto_Prescription_App/Medical_Records.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="885" yWindow="1515" windowWidth="14010" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -52,10 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,25 +452,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="9.85546875" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="5.5703125" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="5.28515625" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
-    <col width="13" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
-    <col width="28.140625" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
-    <col width="26.140625" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
-    <col width="27.140625" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
-    <col width="20.42578125" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="5.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="28.140625" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="20.28515625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="17.28515625" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="2">
+    <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
@@ -594,6 +593,174 @@
       <c r="H5" t="inlineStr">
         <is>
           <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Simran Bala</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>05-01-2025 22:09:18</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ADHD</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>attention deficiet stuff</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Yes yes yes yes yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Subhra Bala</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>05-01-2025 22:32:23</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Eye pain, Heart Ache</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Uterus problem</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Guddu</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>06-01-2025 22:54:52</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Yes yes</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>No NO</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Souradip Banerjee</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>08-01-2025 18:12:44</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Gastritis with sugar problem</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Heart infection</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Covid-20 Checkup</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>eat healthy and workout</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
made some slight adjustments to the LLDB database
</commit_message>
<xml_diff>
--- a/Auto_Prescription_App/Medical_Records.xlsx
+++ b/Auto_Prescription_App/Medical_Records.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
@@ -764,6 +764,90 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Hero Pulsur</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>08-01-2025 20:59:27</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>working</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>working</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>working</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>working</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Swapnanil Bala</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>08-01-2025 21:00:59</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>not</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>working</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>yet</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Added a Bunch of new files
</commit_message>
<xml_diff>
--- a/Auto_Prescription_App/Medical_Records.xlsx
+++ b/Auto_Prescription_App/Medical_Records.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
@@ -848,6 +848,48 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Mahatab Ali</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>16-01-2025 23:05:10</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>pain right groin for last 3 days with fever.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Anterior hip point(right) tender</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>TC DC ESR, Hb, CRP</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Tablet CETIL 250 mg 1 tab BDPC X 5 days.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>